<commit_message>
Working Fp16 and Fp8 code
</commit_message>
<xml_diff>
--- a/result_fp16-LONG_CONTEXT/meta-llama/Meta-Llama-3-8B.xlsx
+++ b/result_fp16-LONG_CONTEXT/meta-llama/Meta-Llama-3-8B.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AH11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -720,10 +720,10 @@
         <v>1024</v>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>1024</v>
@@ -732,67 +732,67 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>5543320</v>
+        <v>3104160</v>
       </c>
       <c r="I3" t="n">
-        <v>0.184727</v>
+        <v>0.32988</v>
       </c>
       <c r="J3" t="n">
-        <v>184.727</v>
+        <v>329.88</v>
       </c>
       <c r="K3" t="n">
-        <v>43305.4</v>
+        <v>96979.3</v>
       </c>
       <c r="L3" t="n">
-        <v>56869.7</v>
+        <v>154990</v>
       </c>
       <c r="M3" t="n">
-        <v>30051.5</v>
+        <v>39562.4</v>
       </c>
       <c r="N3" t="n">
-        <v>43494.9</v>
+        <v>135916</v>
       </c>
       <c r="O3" t="n">
-        <v>43342.3</v>
+        <v>97063.7</v>
       </c>
       <c r="P3" t="n">
-        <v>43301.9</v>
+        <v>96993.7</v>
       </c>
       <c r="Q3" t="n">
-        <v>3484.29</v>
+        <v>4049.02</v>
       </c>
       <c r="R3" t="n">
-        <v>17100.5</v>
+        <v>61339.5</v>
       </c>
       <c r="S3" t="n">
-        <v>2441.44</v>
+        <v>2254.1</v>
       </c>
       <c r="T3" t="n">
-        <v>3662.22</v>
+        <v>42596.9</v>
       </c>
       <c r="U3" t="n">
-        <v>3629.36</v>
+        <v>3204.9</v>
       </c>
       <c r="V3" t="n">
-        <v>3620.27</v>
+        <v>3196.08</v>
       </c>
       <c r="W3" t="n">
-        <v>39.861</v>
+        <v>93.0234</v>
       </c>
       <c r="X3" t="n">
-        <v>40.9932</v>
+        <v>94.86620000000001</v>
       </c>
       <c r="Y3" t="n">
-        <v>26.454</v>
+        <v>36.3991</v>
       </c>
       <c r="Z3" t="n">
-        <v>40.8698</v>
+        <v>94.74039999999999</v>
       </c>
       <c r="AA3" t="n">
-        <v>40.7987</v>
+        <v>93.9936</v>
       </c>
       <c r="AB3" t="n">
-        <v>39.8047</v>
+        <v>93.9012</v>
       </c>
       <c r="AC3" t="n">
         <v>0</v>
@@ -801,16 +801,848 @@
         <v>100</v>
       </c>
       <c r="AE3" t="n">
-        <v>99.06370620198614</v>
+        <v>99.19873291097032</v>
       </c>
       <c r="AF3" t="n">
         <v>0.01708984375</v>
       </c>
       <c r="AG3" t="n">
+        <v>94.796142578125</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>94.34517845466718</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>20002</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D4" t="n">
+        <v>64</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1024</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2993750</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.342046</v>
+      </c>
+      <c r="J4" t="n">
+        <v>342.046</v>
+      </c>
+      <c r="K4" t="n">
+        <v>185724</v>
+      </c>
+      <c r="L4" t="n">
+        <v>318497</v>
+      </c>
+      <c r="M4" t="n">
+        <v>87302.89999999999</v>
+      </c>
+      <c r="N4" t="n">
+        <v>298543</v>
+      </c>
+      <c r="O4" t="n">
+        <v>221640</v>
+      </c>
+      <c r="P4" t="n">
+        <v>174976</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>42024.3</v>
+      </c>
+      <c r="R4" t="n">
+        <v>172260</v>
+      </c>
+      <c r="S4" t="n">
+        <v>2278.46</v>
+      </c>
+      <c r="T4" t="n">
+        <v>152210</v>
+      </c>
+      <c r="U4" t="n">
+        <v>75345.5</v>
+      </c>
+      <c r="V4" t="n">
+        <v>28695</v>
+      </c>
+      <c r="W4" t="n">
+        <v>143.844</v>
+      </c>
+      <c r="X4" t="n">
+        <v>146.91</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>15.2778</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>146.762</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>146.513</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>146.4</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>99.26322156930522</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0.01708984375</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>94.796142578125</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>94.29504563311497</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>20002</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D5" t="n">
+        <v>8</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1024</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4120160</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.248534</v>
+      </c>
+      <c r="J5" t="n">
+        <v>248.534</v>
+      </c>
+      <c r="K5" t="n">
+        <v>32187.4</v>
+      </c>
+      <c r="L5" t="n">
+        <v>44650.2</v>
+      </c>
+      <c r="M5" t="n">
+        <v>19831.6</v>
+      </c>
+      <c r="N5" t="n">
+        <v>32228.4</v>
+      </c>
+      <c r="O5" t="n">
+        <v>32207.8</v>
+      </c>
+      <c r="P5" t="n">
+        <v>32186.5</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>3150.31</v>
+      </c>
+      <c r="R5" t="n">
+        <v>15723.8</v>
+      </c>
+      <c r="S5" t="n">
+        <v>2323.52</v>
+      </c>
+      <c r="T5" t="n">
+        <v>3243.75</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3239.19</v>
+      </c>
+      <c r="V5" t="n">
+        <v>3234.92</v>
+      </c>
+      <c r="W5" t="n">
+        <v>29.0661</v>
+      </c>
+      <c r="X5" t="n">
+        <v>29.8893</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>16.6092</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>29.8742</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>29.8431</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>29.0131</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>99.08427815570673</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.01708984375</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>94.793701171875</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>94.40594201005057</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>20002</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D6" t="n">
+        <v>16</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1024</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4652700</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.220087</v>
+      </c>
+      <c r="J6" t="n">
+        <v>220.087</v>
+      </c>
+      <c r="K6" t="n">
+        <v>72690.60000000001</v>
+      </c>
+      <c r="L6" t="n">
+        <v>103740</v>
+      </c>
+      <c r="M6" t="n">
+        <v>42454.1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>81693.39999999999</v>
+      </c>
+      <c r="O6" t="n">
+        <v>72769.10000000001</v>
+      </c>
+      <c r="P6" t="n">
+        <v>72696.60000000001</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>3775</v>
+      </c>
+      <c r="R6" t="n">
+        <v>34543.4</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2439.15</v>
+      </c>
+      <c r="T6" t="n">
+        <v>12939.6</v>
+      </c>
+      <c r="U6" t="n">
+        <v>3675.19</v>
+      </c>
+      <c r="V6" t="n">
+        <v>3666.02</v>
+      </c>
+      <c r="W6" t="n">
+        <v>68.9846</v>
+      </c>
+      <c r="X6" t="n">
+        <v>70.29689999999999</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>38.8203</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>70.2615</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>69.312</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>69.15049999999999</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>99.53949129852744</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0.01708984375</v>
+      </c>
+      <c r="AG6" t="n">
         <v>95.218505859375</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AH6" t="n">
+        <v>94.85996857438434</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>20002</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D7" t="n">
+        <v>16</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1024</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3446040</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.297153</v>
+      </c>
+      <c r="J7" t="n">
+        <v>297.153</v>
+      </c>
+      <c r="K7" t="n">
+        <v>53839</v>
+      </c>
+      <c r="L7" t="n">
+        <v>81185.10000000001</v>
+      </c>
+      <c r="M7" t="n">
+        <v>26947.2</v>
+      </c>
+      <c r="N7" t="n">
+        <v>61850</v>
+      </c>
+      <c r="O7" t="n">
+        <v>53880.4</v>
+      </c>
+      <c r="P7" t="n">
+        <v>53833</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>3275.67</v>
+      </c>
+      <c r="R7" t="n">
+        <v>30399.5</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2241.93</v>
+      </c>
+      <c r="T7" t="n">
+        <v>11496.2</v>
+      </c>
+      <c r="U7" t="n">
+        <v>3150.19</v>
+      </c>
+      <c r="V7" t="n">
+        <v>3144.42</v>
+      </c>
+      <c r="W7" t="n">
+        <v>50.614</v>
+      </c>
+      <c r="X7" t="n">
+        <v>51.6742</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>23.8249</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>51.6136</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>50.8493</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>50.7781</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>99.13804511278197</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.01708984375</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>94.793701171875</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>94.35730017181626</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>20002</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D8" t="n">
+        <v>64</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1024</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4376010</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.234003</v>
+      </c>
+      <c r="J8" t="n">
+        <v>234.003</v>
+      </c>
+      <c r="K8" t="n">
+        <v>268348</v>
+      </c>
+      <c r="L8" t="n">
+        <v>329773</v>
+      </c>
+      <c r="M8" t="n">
+        <v>96749.10000000001</v>
+      </c>
+      <c r="N8" t="n">
+        <v>307667</v>
+      </c>
+      <c r="O8" t="n">
+        <v>284025</v>
+      </c>
+      <c r="P8" t="n">
+        <v>282935</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>173575</v>
+      </c>
+      <c r="R8" t="n">
+        <v>234509</v>
+      </c>
+      <c r="S8" t="n">
+        <v>2440.02</v>
+      </c>
+      <c r="T8" t="n">
+        <v>212403</v>
+      </c>
+      <c r="U8" t="n">
+        <v>188401</v>
+      </c>
+      <c r="V8" t="n">
+        <v>187509</v>
+      </c>
+      <c r="W8" t="n">
+        <v>94.86799999999999</v>
+      </c>
+      <c r="X8" t="n">
+        <v>96.0693</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>32.7817</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>96.0408</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>95.73439999999999</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>95.5522</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>99.54205164652926</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0.01708984375</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>95.218505859375</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>94.77541780957564</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>20002</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D9" t="n">
+        <v>32</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1024</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4376230</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.233991</v>
+      </c>
+      <c r="J9" t="n">
+        <v>233.991</v>
+      </c>
+      <c r="K9" t="n">
+        <v>136018</v>
+      </c>
+      <c r="L9" t="n">
+        <v>212438</v>
+      </c>
+      <c r="M9" t="n">
+        <v>54874.5</v>
+      </c>
+      <c r="N9" t="n">
+        <v>165970</v>
+      </c>
+      <c r="O9" t="n">
+        <v>165410</v>
+      </c>
+      <c r="P9" t="n">
+        <v>118617</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>41239.8</v>
+      </c>
+      <c r="R9" t="n">
+        <v>117006</v>
+      </c>
+      <c r="S9" t="n">
+        <v>2434.27</v>
+      </c>
+      <c r="T9" t="n">
+        <v>70506.8</v>
+      </c>
+      <c r="U9" t="n">
+        <v>69950.7</v>
+      </c>
+      <c r="V9" t="n">
+        <v>22997.2</v>
+      </c>
+      <c r="W9" t="n">
+        <v>94.8729</v>
+      </c>
+      <c r="X9" t="n">
+        <v>96.0656</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>32.7835</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>96.04819999999999</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>95.7333</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>95.55</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>99.5798578199052</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0.01708984375</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>95.218505859375</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>94.79732770151436</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>20002</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1024</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>5543320</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.184727</v>
+      </c>
+      <c r="J10" t="n">
+        <v>184.727</v>
+      </c>
+      <c r="K10" t="n">
+        <v>43305.4</v>
+      </c>
+      <c r="L10" t="n">
+        <v>56869.7</v>
+      </c>
+      <c r="M10" t="n">
+        <v>30051.5</v>
+      </c>
+      <c r="N10" t="n">
+        <v>43494.9</v>
+      </c>
+      <c r="O10" t="n">
+        <v>43342.3</v>
+      </c>
+      <c r="P10" t="n">
+        <v>43301.9</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>3484.29</v>
+      </c>
+      <c r="R10" t="n">
+        <v>17100.5</v>
+      </c>
+      <c r="S10" t="n">
+        <v>2441.44</v>
+      </c>
+      <c r="T10" t="n">
+        <v>3662.22</v>
+      </c>
+      <c r="U10" t="n">
+        <v>3629.36</v>
+      </c>
+      <c r="V10" t="n">
+        <v>3620.27</v>
+      </c>
+      <c r="W10" t="n">
+        <v>39.861</v>
+      </c>
+      <c r="X10" t="n">
+        <v>40.9932</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>26.454</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>40.8698</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>40.7987</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>39.8047</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>99.06370620198614</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0.01708984375</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>95.218505859375</v>
+      </c>
+      <c r="AH10" t="n">
         <v>94.86421147289852</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>20002</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1024</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7444400</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.137553</v>
+      </c>
+      <c r="J11" t="n">
+        <v>137.553</v>
+      </c>
+      <c r="K11" t="n">
+        <v>14539.7</v>
+      </c>
+      <c r="L11" t="n">
+        <v>15210.7</v>
+      </c>
+      <c r="M11" t="n">
+        <v>13877.6</v>
+      </c>
+      <c r="N11" t="n">
+        <v>14552.5</v>
+      </c>
+      <c r="O11" t="n">
+        <v>14546.6</v>
+      </c>
+      <c r="P11" t="n">
+        <v>14540.2</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2671.52</v>
+      </c>
+      <c r="R11" t="n">
+        <v>3751.09</v>
+      </c>
+      <c r="S11" t="n">
+        <v>2226.43</v>
+      </c>
+      <c r="T11" t="n">
+        <v>3096.77</v>
+      </c>
+      <c r="U11" t="n">
+        <v>3095.37</v>
+      </c>
+      <c r="V11" t="n">
+        <v>2250.74</v>
+      </c>
+      <c r="W11" t="n">
+        <v>11.88</v>
+      </c>
+      <c r="X11" t="n">
+        <v>12.3239</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>10.7941</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>12.3158</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>12.3084</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>11.4763</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>98.33391657334826</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0.01708984375</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>94.793701171875</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>94.60316281035659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>